<commit_message>
final submission week3, also adjusted previous weeks' files
</commit_message>
<xml_diff>
--- a/quizzes/week3/w3_calcs.xlsx
+++ b/quizzes/week3/w3_calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amanj\ds_projects\unsw\decision_making_6510\quizzes\week3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8A4240-2B9B-4540-88ED-31C1DF1F4889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56BA021-59D1-4679-B9D9-7294415B616B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{0F7E80EF-D48E-4510-842D-75B7F8EC6273}"/>
   </bookViews>
@@ -161,8 +161,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="170" formatCode="0.0000"/>
-    <numFmt numFmtId="171" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -370,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -381,10 +381,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -399,31 +399,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -441,31 +441,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -474,14 +474,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -489,11 +483,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5198,10 +5189,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9EF158-2029-44A9-8CA7-93AC60014193}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5216,8 +5207,8 @@
     <col min="10" max="10" width="11.08203125" style="3" customWidth="1"/>
     <col min="11" max="11" width="14.58203125" style="3" customWidth="1"/>
     <col min="12" max="12" width="8.6640625" style="3"/>
-    <col min="13" max="2000" width="8.6640625" style="2"/>
-    <col min="2001" max="2001" width="2.4140625" style="2" customWidth="1"/>
+    <col min="13" max="1999" width="8.6640625" style="2"/>
+    <col min="2000" max="2001" width="2.4140625" style="2" customWidth="1"/>
     <col min="2002" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
@@ -5822,11 +5813,11 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B34" s="1" t="s">
         <v>4</v>
       </c>
@@ -5843,7 +5834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" ht="17.5" x14ac:dyDescent="0.35">
       <c r="C35" s="16" t="s">
         <v>0</v>
       </c>
@@ -5863,7 +5854,7 @@
         <v>3.0958034099089407</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C36" s="19" t="s">
         <v>1</v>
       </c>
@@ -5883,7 +5874,7 @@
         <v>4.7901704954470326E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C37" s="20" t="s">
         <v>2</v>
       </c>
@@ -5903,7 +5894,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
       <c r="H38" s="22" t="s">
         <v>18</v>
       </c>
@@ -5912,7 +5903,7 @@
         <v>8.2589146473224712E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
       <c r="H39" s="6" t="s">
         <v>22</v>
       </c>
@@ -5921,7 +5912,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B41" s="1" t="s">
         <v>0</v>
       </c>
@@ -5938,7 +5929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="2:11" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" ht="17.5" x14ac:dyDescent="0.35">
       <c r="C42" s="16" t="s">
         <v>5</v>
       </c>
@@ -5953,12 +5944,12 @@
       <c r="H42" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I42" s="36">
+      <c r="I42" s="35">
         <f>AVERAGE(E42:E44)</f>
         <v>3.0183672246175566</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C43" s="19" t="s">
         <v>6</v>
       </c>
@@ -5973,13 +5964,12 @@
       <c r="H43" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I43" s="36">
+      <c r="I43" s="35">
         <f>(I42-I41)/(I41-1)</f>
         <v>9.1836123087782884E-3</v>
       </c>
-      <c r="K43" s="37"/>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C44" s="20" t="s">
         <v>3</v>
       </c>
@@ -5994,30 +5984,30 @@
       <c r="H44" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I44" s="36">
+      <c r="I44" s="35">
         <f>0.58</f>
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
       <c r="H45" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="I45" s="36">
+      <c r="I45" s="35">
         <f>I43/I44</f>
         <v>1.5833814325479808E-2</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
       <c r="H46" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I46" s="38" t="str">
+      <c r="I46" s="36" t="str">
         <f>IF(I45&lt;=0.1, "Yes", "No")</f>
         <v>Yes</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B48" s="1" t="s">
         <v>1</v>
       </c>
@@ -6049,7 +6039,7 @@
       <c r="H49" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I49" s="36">
+      <c r="I49" s="35">
         <f>AVERAGE(E49:E51)</f>
         <v>3.0183247941395699</v>
       </c>
@@ -6069,7 +6059,7 @@
       <c r="H50" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I50" s="36">
+      <c r="I50" s="35">
         <f>(I49-I48)/(I48-1)</f>
         <v>9.1623970697849444E-3</v>
       </c>
@@ -6089,7 +6079,7 @@
       <c r="H51" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I51" s="36">
+      <c r="I51" s="35">
         <f>0.58</f>
         <v>0.57999999999999996</v>
       </c>
@@ -6098,7 +6088,7 @@
       <c r="H52" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="I52" s="36">
+      <c r="I52" s="35">
         <f>I50/I51</f>
         <v>1.5797236327215424E-2</v>
       </c>
@@ -6107,7 +6097,7 @@
       <c r="H53" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I53" s="38" t="str">
+      <c r="I53" s="36" t="str">
         <f>IF(I52&lt;=0.1, "Yes", "No")</f>
         <v>Yes</v>
       </c>
@@ -6144,7 +6134,7 @@
       <c r="H56" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I56" s="36">
+      <c r="I56" s="35">
         <f>AVERAGE(E56:E58)</f>
         <v>3.053901203220224</v>
       </c>
@@ -6164,7 +6154,7 @@
       <c r="H57" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I57" s="36">
+      <c r="I57" s="35">
         <f>(I56-I55)/(I55-1)</f>
         <v>2.6950601610111979E-2</v>
       </c>
@@ -6184,7 +6174,7 @@
       <c r="H58" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I58" s="36">
+      <c r="I58" s="35">
         <f>0.58</f>
         <v>0.57999999999999996</v>
       </c>
@@ -6193,7 +6183,7 @@
       <c r="H59" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="I59" s="36">
+      <c r="I59" s="35">
         <f>I57/I58</f>
         <v>4.6466554500193068E-2</v>
       </c>
@@ -6202,7 +6192,7 @@
       <c r="H60" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I60" s="38" t="str">
+      <c r="I60" s="36" t="str">
         <f>IF(I59&lt;=0.1, "Yes", "No")</f>
         <v>Yes</v>
       </c>
@@ -6218,7 +6208,7 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D64" s="39" t="s">
+      <c r="D64" s="37" t="s">
         <v>25</v>
       </c>
     </row>
@@ -6253,7 +6243,7 @@
       <c r="C68" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D68" s="40" t="str">
+      <c r="D68" s="38" t="str">
         <f>_xlfn.XLOOKUP(MAX(D65:D67),D65:D67,C65:C67)</f>
         <v>Coaxial</v>
       </c>
@@ -6267,9 +6257,6 @@
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D72" s="4"/>
-    </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C73" s="41"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I39 I46 I53 I60">

</xml_diff>